<commit_message>
cost center API Test cases updating
</commit_message>
<xml_diff>
--- a/tests/artifact/script/CostCenterAPI.xlsx
+++ b/tests/artifact/script/CostCenterAPI.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9024" tabRatio="500" firstSheet="3" activeTab="3"/>
+    <workbookView windowWidth="23040" windowHeight="9024" tabRatio="500" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2049" uniqueCount="955">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2049" uniqueCount="954">
   <si>
     <t>target</t>
   </si>
@@ -2624,7 +2624,7 @@
 expectedReturnCode=200
 expectedResponseTime=3000
 expectedContentType=application/json
-schema=${schema.path}\DeliveryNote.txt</t>
+schema=${schema.path}\CostCenter.txt</t>
   </si>
   <si>
     <t>validating the success to the actual status</t>
@@ -3101,16 +3101,6 @@
   </si>
   <si>
     <t>Positive - /CostCenter/delchal</t>
-  </si>
-  <si>
-    <t>actualReturnCode=${response}.returnCode
-actualResponseTime=${response}.elapsedTime
-actualContentType=${response}.headers.[Content-Type]
-responseBody=${response}.body
-expectedReturnCode=200
-expectedResponseTime=3000
-expectedContentType=application/json
-schema=${schema.path}\CostCenter.txt</t>
   </si>
   <si>
     <t>Create CostCenter for product: POST- /CostCenter</t>
@@ -7861,10 +7851,10 @@
     </row>
     <row r="6" s="4" customFormat="1" customHeight="1" spans="1:15">
       <c r="A6" s="28" t="s">
+        <v>937</v>
+      </c>
+      <c r="B6" s="19" t="s">
         <v>938</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>939</v>
       </c>
       <c r="C6" s="20" t="s">
         <v>5</v>
@@ -7876,7 +7866,7 @@
         <v>783</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="G6" s="19"/>
       <c r="H6" s="29"/>
@@ -7891,7 +7881,7 @@
     <row r="7" s="4" customFormat="1" customHeight="1" spans="1:15">
       <c r="A7" s="18"/>
       <c r="B7" s="19" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="C7" s="20" t="s">
         <v>35</v>
@@ -7998,10 +7988,10 @@
     </row>
     <row r="11" s="1" customFormat="1" customHeight="1" spans="1:15">
       <c r="A11" s="18" t="s">
+        <v>939</v>
+      </c>
+      <c r="B11" s="19" t="s">
         <v>940</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>941</v>
       </c>
       <c r="C11" s="20" t="s">
         <v>5</v>
@@ -8013,7 +8003,7 @@
         <v>783</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="G11" s="26"/>
       <c r="H11" s="26"/>
@@ -8028,7 +8018,7 @@
     <row r="12" s="1" customFormat="1" customHeight="1" spans="1:15">
       <c r="A12" s="18"/>
       <c r="B12" s="19" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="C12" s="20" t="s">
         <v>35</v>
@@ -8055,7 +8045,7 @@
     <row r="13" s="1" customFormat="1" customHeight="1" spans="1:15">
       <c r="A13" s="18"/>
       <c r="B13" s="19" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="C13" s="20" t="s">
         <v>5</v>
@@ -8080,7 +8070,7 @@
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:15">
       <c r="A14" s="18"/>
       <c r="B14" s="19" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="C14" s="20" t="s">
         <v>5</v>
@@ -8107,7 +8097,7 @@
     <row r="15" s="1" customFormat="1" customHeight="1" spans="1:15">
       <c r="A15" s="18"/>
       <c r="B15" s="19" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="C15" s="20" t="s">
         <v>5</v>
@@ -8116,10 +8106,10 @@
         <v>471</v>
       </c>
       <c r="E15" s="19" t="s">
+        <v>946</v>
+      </c>
+      <c r="F15" s="19" t="s">
         <v>947</v>
-      </c>
-      <c r="F15" s="19" t="s">
-        <v>948</v>
       </c>
       <c r="G15" s="26"/>
       <c r="H15" s="26"/>
@@ -8160,10 +8150,10 @@
     </row>
     <row r="17" s="1" customFormat="1" customHeight="1" spans="1:15">
       <c r="A17" s="33" t="s">
+        <v>948</v>
+      </c>
+      <c r="B17" s="26" t="s">
         <v>949</v>
-      </c>
-      <c r="B17" s="26" t="s">
-        <v>950</v>
       </c>
       <c r="C17" s="25" t="s">
         <v>5</v>
@@ -8175,7 +8165,7 @@
         <v>783</v>
       </c>
       <c r="F17" s="26" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="G17" s="26"/>
       <c r="H17" s="19"/>
@@ -8190,7 +8180,7 @@
     <row r="18" s="1" customFormat="1" customHeight="1" spans="1:15">
       <c r="A18" s="33"/>
       <c r="B18" s="26" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="C18" s="25" t="s">
         <v>35</v>
@@ -8217,7 +8207,7 @@
     <row r="19" s="1" customFormat="1" customHeight="1" spans="1:15">
       <c r="A19" s="33"/>
       <c r="B19" s="34" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="C19" s="25" t="s">
         <v>5</v>
@@ -8242,7 +8232,7 @@
     <row r="20" s="1" customFormat="1" customHeight="1" spans="1:15">
       <c r="A20" s="33"/>
       <c r="B20" s="19" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="C20" s="20" t="s">
         <v>5</v>
@@ -8295,10 +8285,10 @@
     </row>
     <row r="22" s="1" customFormat="1" customHeight="1" spans="1:15">
       <c r="A22" s="33" t="s">
+        <v>952</v>
+      </c>
+      <c r="B22" s="26" t="s">
         <v>953</v>
-      </c>
-      <c r="B22" s="26" t="s">
-        <v>954</v>
       </c>
       <c r="C22" s="25" t="s">
         <v>5</v>
@@ -8310,7 +8300,7 @@
         <v>783</v>
       </c>
       <c r="F22" s="26" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="G22" s="26"/>
       <c r="H22" s="19"/>
@@ -8325,7 +8315,7 @@
     <row r="23" s="1" customFormat="1" customHeight="1" spans="1:15">
       <c r="A23" s="33"/>
       <c r="B23" s="26" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="C23" s="25" t="s">
         <v>35</v>
@@ -8352,7 +8342,7 @@
     <row r="24" s="1" customFormat="1" customHeight="1" spans="1:15">
       <c r="A24" s="33"/>
       <c r="B24" s="34" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="C24" s="25" t="s">
         <v>5</v>
@@ -8377,7 +8367,7 @@
     <row r="25" s="1" customFormat="1" customHeight="1" spans="1:15">
       <c r="A25" s="33"/>
       <c r="B25" s="19" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="C25" s="20" t="s">
         <v>5</v>
@@ -31497,8 +31487,8 @@
   <sheetPr/>
   <dimension ref="A1:O142"/>
   <sheetViews>
-    <sheetView zoomScale="77" zoomScaleNormal="77" topLeftCell="B20" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="24" customHeight="1"/>
@@ -34601,8 +34591,8 @@
   <sheetPr/>
   <dimension ref="A1:O130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="13.8"/>
@@ -34847,7 +34837,7 @@
       <c r="N8" s="21"/>
       <c r="O8" s="19"/>
     </row>
-    <row r="9" s="1" customFormat="1" ht="27.6" spans="1:15">
+    <row r="9" s="1" customFormat="1" ht="248.4" spans="1:15">
       <c r="A9" s="18"/>
       <c r="B9" s="51" t="s">
         <v>826</v>
@@ -34861,7 +34851,7 @@
       <c r="E9" s="19" t="s">
         <v>800</v>
       </c>
-      <c r="F9" s="19" t="s">
+      <c r="F9" s="30" t="s">
         <v>841</v>
       </c>
       <c r="G9" s="19"/>
@@ -46079,7 +46069,7 @@
         <v>800</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>917</v>
+        <v>841</v>
       </c>
       <c r="G10" s="19"/>
       <c r="H10" s="19"/>
@@ -46120,7 +46110,7 @@
     </row>
     <row r="12" s="53" customFormat="1" customHeight="1" spans="1:25">
       <c r="A12" s="23" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="B12" s="19" t="s">
         <v>768</v>
@@ -46282,7 +46272,7 @@
         <v>800</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>917</v>
+        <v>841</v>
       </c>
       <c r="G17" s="19"/>
       <c r="H17" s="29"/>
@@ -46296,7 +46286,7 @@
     </row>
     <row r="18" s="82" customFormat="1" customHeight="1" spans="1:15">
       <c r="A18" s="23" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="B18" s="19" t="s">
         <v>768</v>
@@ -46421,7 +46411,7 @@
         <v>800</v>
       </c>
       <c r="F22" s="30" t="s">
-        <v>917</v>
+        <v>841</v>
       </c>
       <c r="G22" s="19"/>
       <c r="H22" s="19"/>
@@ -49546,10 +49536,10 @@
     </row>
     <row r="6" s="54" customFormat="1" customHeight="1" spans="1:15">
       <c r="A6" s="66" t="s">
+        <v>919</v>
+      </c>
+      <c r="B6" s="67" t="s">
         <v>920</v>
-      </c>
-      <c r="B6" s="67" t="s">
-        <v>921</v>
       </c>
       <c r="C6" s="68" t="s">
         <v>5</v>
@@ -49576,7 +49566,7 @@
     <row r="7" s="55" customFormat="1" customHeight="1" spans="1:15">
       <c r="A7" s="66"/>
       <c r="B7" s="72" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="C7" s="59" t="s">
         <v>5</v>
@@ -49588,7 +49578,7 @@
         <v>873</v>
       </c>
       <c r="F7" s="67" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="G7" s="67"/>
       <c r="H7" s="67"/>
@@ -49603,7 +49593,7 @@
     <row r="8" s="54" customFormat="1" customHeight="1" spans="1:15">
       <c r="A8" s="66"/>
       <c r="B8" s="67" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="C8" s="68" t="s">
         <v>35</v>
@@ -49712,7 +49702,7 @@
     </row>
     <row r="12" s="54" customFormat="1" customHeight="1" spans="1:15">
       <c r="A12" s="66" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="B12" s="26" t="s">
         <v>815</v>
@@ -49742,7 +49732,7 @@
     <row r="13" s="55" customFormat="1" customHeight="1" spans="1:15">
       <c r="A13" s="73"/>
       <c r="B13" s="72" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="C13" s="59" t="s">
         <v>5</v>
@@ -49754,7 +49744,7 @@
         <v>873</v>
       </c>
       <c r="F13" s="74" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="G13" s="67"/>
       <c r="H13" s="67"/>
@@ -49769,7 +49759,7 @@
     <row r="14" s="54" customFormat="1" customHeight="1" spans="1:15">
       <c r="A14" s="66"/>
       <c r="B14" s="67" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="C14" s="68" t="s">
         <v>35</v>
@@ -49878,7 +49868,7 @@
     </row>
     <row r="18" s="54" customFormat="1" customHeight="1" spans="1:15">
       <c r="A18" s="66" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="B18" s="26" t="s">
         <v>815</v>
@@ -49908,7 +49898,7 @@
     <row r="19" s="55" customFormat="1" customHeight="1" spans="1:15">
       <c r="A19" s="75"/>
       <c r="B19" s="72" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="C19" s="59" t="s">
         <v>5</v>
@@ -49920,7 +49910,7 @@
         <v>873</v>
       </c>
       <c r="F19" s="67" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="G19" s="67"/>
       <c r="H19" s="67"/>
@@ -49935,7 +49925,7 @@
     <row r="20" s="54" customFormat="1" customHeight="1" spans="1:15">
       <c r="A20" s="66"/>
       <c r="B20" s="67" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="C20" s="68" t="s">
         <v>35</v>
@@ -50044,7 +50034,7 @@
     </row>
     <row r="24" s="54" customFormat="1" customHeight="1" spans="1:15">
       <c r="A24" s="66" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="B24" s="26" t="s">
         <v>815</v>
@@ -50074,7 +50064,7 @@
     <row r="25" s="55" customFormat="1" customHeight="1" spans="1:15">
       <c r="A25" s="75"/>
       <c r="B25" s="72" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="C25" s="59" t="s">
         <v>5</v>
@@ -50086,7 +50076,7 @@
         <v>873</v>
       </c>
       <c r="F25" s="67" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="G25" s="67"/>
       <c r="H25" s="67"/>
@@ -50101,7 +50091,7 @@
     <row r="26" s="54" customFormat="1" customHeight="1" spans="1:15">
       <c r="A26" s="66"/>
       <c r="B26" s="67" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="C26" s="68" t="s">
         <v>35</v>
@@ -50210,7 +50200,7 @@
     </row>
     <row r="30" s="54" customFormat="1" customHeight="1" spans="1:15">
       <c r="A30" s="66" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="B30" s="26" t="s">
         <v>815</v>
@@ -50240,7 +50230,7 @@
     <row r="31" s="55" customFormat="1" customHeight="1" spans="1:15">
       <c r="A31" s="75"/>
       <c r="B31" s="72" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="C31" s="59" t="s">
         <v>5</v>
@@ -50252,7 +50242,7 @@
         <v>873</v>
       </c>
       <c r="F31" s="74" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="G31" s="67"/>
       <c r="H31" s="67"/>
@@ -50267,7 +50257,7 @@
     <row r="32" s="54" customFormat="1" customHeight="1" spans="1:15">
       <c r="A32" s="66"/>
       <c r="B32" s="67" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="C32" s="68" t="s">
         <v>35</v>
@@ -53287,7 +53277,7 @@
     <row r="8" s="1" customFormat="1" customHeight="1" spans="1:15">
       <c r="A8" s="18"/>
       <c r="B8" s="19" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="C8" s="20" t="s">
         <v>35</v>
@@ -53355,7 +53345,7 @@
         <v>800</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>917</v>
+        <v>841</v>
       </c>
       <c r="G10" s="19"/>
       <c r="H10" s="19"/>
@@ -53396,7 +53386,7 @@
     </row>
     <row r="12" s="4" customFormat="1" customHeight="1" spans="1:15">
       <c r="A12" s="18" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="B12" s="26" t="s">
         <v>815</v>
@@ -53411,7 +53401,7 @@
         <v>783</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="G12" s="19"/>
       <c r="H12" s="29"/>
@@ -53426,7 +53416,7 @@
     <row r="13" s="1" customFormat="1" customHeight="1" spans="1:15">
       <c r="A13" s="18"/>
       <c r="B13" s="19" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="C13" s="20" t="s">
         <v>35</v>
@@ -53492,7 +53482,7 @@
         <v>800</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>917</v>
+        <v>841</v>
       </c>
       <c r="G15" s="19"/>
       <c r="H15" s="19"/>
@@ -53543,7 +53533,7 @@
         <v>107</v>
       </c>
       <c r="E17" s="26" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>

</xml_diff>